<commit_message>
change the random seed & delete unnecessary files
</commit_message>
<xml_diff>
--- a/full_customers.xlsx
+++ b/full_customers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ztlu\Documents\MMA Code\RBAC-Calian-Case-Competition\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utoronto-my.sharepoint.com/personal/kyrie_xu_rotman_utoronto_ca/Documents/MMA/Calian-case-competition/RBAC-Calian-Case-Competition/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{7B3A9A0D-A81A-4396-BB78-BC87382B7D79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{076A3304-1A31-4749-8B5E-E43EEEABE8B9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{076A3304-1A31-4749-8B5E-E43EEEABE8B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5491,9 +5491,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5830,16 +5830,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CECBB19-2994-4C7F-AD6F-F5F68BAE70BA}">
   <dimension ref="A1:K501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A475" workbookViewId="0">
-      <selection activeCell="J488" sqref="J488"/>
+    <sheetView tabSelected="1" topLeftCell="A219" workbookViewId="0">
+      <selection activeCell="A246" sqref="A246"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5874,7 +5874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -5909,7 +5909,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
@@ -5944,7 +5944,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
@@ -5979,7 +5979,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>30</v>
       </c>
@@ -6014,7 +6014,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>35</v>
       </c>
@@ -6049,7 +6049,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>40</v>
       </c>
@@ -6084,7 +6084,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>44</v>
       </c>
@@ -6119,7 +6119,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>49</v>
       </c>
@@ -6154,7 +6154,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>54</v>
       </c>
@@ -6189,7 +6189,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>58</v>
       </c>
@@ -6224,7 +6224,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>62</v>
       </c>
@@ -6259,7 +6259,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>67</v>
       </c>
@@ -6294,7 +6294,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>71</v>
       </c>
@@ -6329,7 +6329,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>76</v>
       </c>
@@ -6364,7 +6364,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>80</v>
       </c>
@@ -6399,7 +6399,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>85</v>
       </c>
@@ -6434,7 +6434,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>89</v>
       </c>
@@ -6469,7 +6469,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>94</v>
       </c>
@@ -6504,7 +6504,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>98</v>
       </c>
@@ -6539,7 +6539,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>103</v>
       </c>
@@ -6574,7 +6574,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>108</v>
       </c>
@@ -6609,7 +6609,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>112</v>
       </c>
@@ -6644,7 +6644,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>117</v>
       </c>
@@ -6679,7 +6679,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>121</v>
       </c>
@@ -6714,7 +6714,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>125</v>
       </c>
@@ -6749,7 +6749,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>129</v>
       </c>
@@ -6784,7 +6784,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>134</v>
       </c>
@@ -6819,7 +6819,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>138</v>
       </c>
@@ -6854,7 +6854,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>142</v>
       </c>
@@ -6889,7 +6889,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>146</v>
       </c>
@@ -6924,7 +6924,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>150</v>
       </c>
@@ -6959,7 +6959,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>154</v>
       </c>
@@ -6994,7 +6994,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>71</v>
       </c>
@@ -7029,7 +7029,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>162</v>
       </c>
@@ -7064,7 +7064,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>166</v>
       </c>
@@ -7099,7 +7099,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>170</v>
       </c>
@@ -7134,7 +7134,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>174</v>
       </c>
@@ -7169,7 +7169,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>178</v>
       </c>
@@ -7204,7 +7204,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>182</v>
       </c>
@@ -7239,7 +7239,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>186</v>
       </c>
@@ -7274,7 +7274,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>190</v>
       </c>
@@ -7309,7 +7309,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>194</v>
       </c>
@@ -7344,7 +7344,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>198</v>
       </c>
@@ -7379,7 +7379,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>203</v>
       </c>
@@ -7414,7 +7414,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>207</v>
       </c>
@@ -7449,7 +7449,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>212</v>
       </c>
@@ -7484,7 +7484,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>216</v>
       </c>
@@ -7519,7 +7519,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>220</v>
       </c>
@@ -7554,7 +7554,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>224</v>
       </c>
@@ -7589,7 +7589,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>228</v>
       </c>
@@ -7624,7 +7624,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>232</v>
       </c>
@@ -7659,7 +7659,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>236</v>
       </c>
@@ -7694,7 +7694,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>240</v>
       </c>
@@ -7729,7 +7729,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>244</v>
       </c>
@@ -7764,7 +7764,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>248</v>
       </c>
@@ -7799,7 +7799,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>252</v>
       </c>
@@ -7834,7 +7834,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>256</v>
       </c>
@@ -7869,7 +7869,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>261</v>
       </c>
@@ -7904,7 +7904,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>265</v>
       </c>
@@ -7939,7 +7939,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>269</v>
       </c>
@@ -7974,7 +7974,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>274</v>
       </c>
@@ -8009,7 +8009,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>278</v>
       </c>
@@ -8044,7 +8044,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>282</v>
       </c>
@@ -8079,7 +8079,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>286</v>
       </c>
@@ -8114,7 +8114,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>290</v>
       </c>
@@ -8149,7 +8149,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>294</v>
       </c>
@@ -8184,7 +8184,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>298</v>
       </c>
@@ -8219,7 +8219,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>302</v>
       </c>
@@ -8254,7 +8254,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>306</v>
       </c>
@@ -8289,7 +8289,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>310</v>
       </c>
@@ -8324,7 +8324,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>314</v>
       </c>
@@ -8359,7 +8359,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>318</v>
       </c>
@@ -8394,7 +8394,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>322</v>
       </c>
@@ -8429,7 +8429,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>326</v>
       </c>
@@ -8464,7 +8464,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>330</v>
       </c>
@@ -8499,7 +8499,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>334</v>
       </c>
@@ -8534,7 +8534,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>338</v>
       </c>
@@ -8569,7 +8569,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>342</v>
       </c>
@@ -8604,7 +8604,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>346</v>
       </c>
@@ -8639,7 +8639,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>350</v>
       </c>
@@ -8674,7 +8674,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>354</v>
       </c>
@@ -8709,7 +8709,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>358</v>
       </c>
@@ -8744,7 +8744,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>362</v>
       </c>
@@ -8779,7 +8779,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>366</v>
       </c>
@@ -8814,7 +8814,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>370</v>
       </c>
@@ -8849,7 +8849,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>374</v>
       </c>
@@ -8884,7 +8884,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>378</v>
       </c>
@@ -8919,7 +8919,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>382</v>
       </c>
@@ -8954,7 +8954,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>386</v>
       </c>
@@ -8989,7 +8989,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>390</v>
       </c>
@@ -9024,7 +9024,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>394</v>
       </c>
@@ -9059,7 +9059,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>398</v>
       </c>
@@ -9094,7 +9094,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>402</v>
       </c>
@@ -9129,7 +9129,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>406</v>
       </c>
@@ -9164,7 +9164,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>410</v>
       </c>
@@ -9199,7 +9199,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>414</v>
       </c>
@@ -9234,7 +9234,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>418</v>
       </c>
@@ -9269,7 +9269,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>422</v>
       </c>
@@ -9304,7 +9304,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>67</v>
       </c>
@@ -9339,7 +9339,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>429</v>
       </c>
@@ -9374,7 +9374,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>433</v>
       </c>
@@ -9409,7 +9409,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>438</v>
       </c>
@@ -9444,7 +9444,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>443</v>
       </c>
@@ -9479,7 +9479,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>447</v>
       </c>
@@ -9514,7 +9514,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>451</v>
       </c>
@@ -9549,7 +9549,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>290</v>
       </c>
@@ -9584,7 +9584,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>458</v>
       </c>
@@ -9619,7 +9619,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>462</v>
       </c>
@@ -9654,7 +9654,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>466</v>
       </c>
@@ -9689,7 +9689,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>470</v>
       </c>
@@ -9724,7 +9724,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>474</v>
       </c>
@@ -9759,7 +9759,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>478</v>
       </c>
@@ -9794,7 +9794,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>482</v>
       </c>
@@ -9829,7 +9829,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>486</v>
       </c>
@@ -9864,7 +9864,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>490</v>
       </c>
@@ -9899,7 +9899,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>494</v>
       </c>
@@ -9934,7 +9934,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>498</v>
       </c>
@@ -9969,7 +9969,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>502</v>
       </c>
@@ -10004,7 +10004,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>506</v>
       </c>
@@ -10039,7 +10039,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>510</v>
       </c>
@@ -10074,7 +10074,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>514</v>
       </c>
@@ -10109,7 +10109,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>518</v>
       </c>
@@ -10144,7 +10144,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>522</v>
       </c>
@@ -10179,7 +10179,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>526</v>
       </c>
@@ -10214,7 +10214,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>530</v>
       </c>
@@ -10249,7 +10249,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>534</v>
       </c>
@@ -10284,7 +10284,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>538</v>
       </c>
@@ -10319,7 +10319,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>542</v>
       </c>
@@ -10354,7 +10354,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>546</v>
       </c>
@@ -10389,7 +10389,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>550</v>
       </c>
@@ -10424,7 +10424,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>554</v>
       </c>
@@ -10459,7 +10459,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>558</v>
       </c>
@@ -10494,7 +10494,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>562</v>
       </c>
@@ -10529,7 +10529,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>566</v>
       </c>
@@ -10564,7 +10564,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>570</v>
       </c>
@@ -10599,7 +10599,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>574</v>
       </c>
@@ -10634,7 +10634,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>578</v>
       </c>
@@ -10669,7 +10669,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>582</v>
       </c>
@@ -10704,7 +10704,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>586</v>
       </c>
@@ -10739,7 +10739,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>590</v>
       </c>
@@ -10774,7 +10774,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>40</v>
       </c>
@@ -10809,7 +10809,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>203</v>
       </c>
@@ -10844,7 +10844,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>600</v>
       </c>
@@ -10879,7 +10879,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>604</v>
       </c>
@@ -10914,7 +10914,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>608</v>
       </c>
@@ -10949,7 +10949,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>612</v>
       </c>
@@ -10984,7 +10984,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>616</v>
       </c>
@@ -11019,7 +11019,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>620</v>
       </c>
@@ -11054,7 +11054,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>624</v>
       </c>
@@ -11089,7 +11089,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>628</v>
       </c>
@@ -11124,7 +11124,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>632</v>
       </c>
@@ -11159,7 +11159,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>224</v>
       </c>
@@ -11194,7 +11194,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>639</v>
       </c>
@@ -11229,7 +11229,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>643</v>
       </c>
@@ -11264,7 +11264,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>647</v>
       </c>
@@ -11299,7 +11299,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>651</v>
       </c>
@@ -11334,7 +11334,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>655</v>
       </c>
@@ -11369,7 +11369,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>659</v>
       </c>
@@ -11404,7 +11404,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>663</v>
       </c>
@@ -11439,7 +11439,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>667</v>
       </c>
@@ -11474,7 +11474,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>671</v>
       </c>
@@ -11509,7 +11509,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>675</v>
       </c>
@@ -11544,7 +11544,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>679</v>
       </c>
@@ -11579,7 +11579,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>684</v>
       </c>
@@ -11614,7 +11614,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>688</v>
       </c>
@@ -11649,7 +11649,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>693</v>
       </c>
@@ -11684,7 +11684,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>697</v>
       </c>
@@ -11719,7 +11719,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>701</v>
       </c>
@@ -11754,7 +11754,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>705</v>
       </c>
@@ -11789,7 +11789,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>709</v>
       </c>
@@ -11824,7 +11824,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>713</v>
       </c>
@@ -11859,7 +11859,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>717</v>
       </c>
@@ -11894,7 +11894,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>721</v>
       </c>
@@ -11929,7 +11929,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
         <v>725</v>
       </c>
@@ -11964,7 +11964,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
         <v>729</v>
       </c>
@@ -11999,7 +11999,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
         <v>733</v>
       </c>
@@ -12034,7 +12034,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
         <v>737</v>
       </c>
@@ -12069,7 +12069,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
         <v>741</v>
       </c>
@@ -12104,7 +12104,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
         <v>745</v>
       </c>
@@ -12139,7 +12139,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
         <v>749</v>
       </c>
@@ -12174,7 +12174,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
         <v>753</v>
       </c>
@@ -12209,7 +12209,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
         <v>757</v>
       </c>
@@ -12244,7 +12244,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
         <v>761</v>
       </c>
@@ -12279,7 +12279,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
         <v>765</v>
       </c>
@@ -12314,7 +12314,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
         <v>769</v>
       </c>
@@ -12349,7 +12349,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
         <v>773</v>
       </c>
@@ -12384,7 +12384,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
         <v>777</v>
       </c>
@@ -12419,7 +12419,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
         <v>781</v>
       </c>
@@ -12454,7 +12454,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
         <v>785</v>
       </c>
@@ -12489,7 +12489,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
         <v>789</v>
       </c>
@@ -12524,7 +12524,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
         <v>256</v>
       </c>
@@ -12559,7 +12559,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
         <v>796</v>
       </c>
@@ -12594,7 +12594,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
         <v>800</v>
       </c>
@@ -12629,7 +12629,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
         <v>804</v>
       </c>
@@ -12664,7 +12664,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
         <v>808</v>
       </c>
@@ -12699,7 +12699,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
         <v>812</v>
       </c>
@@ -12734,7 +12734,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
         <v>816</v>
       </c>
@@ -12769,7 +12769,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
         <v>820</v>
       </c>
@@ -12804,7 +12804,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
         <v>824</v>
       </c>
@@ -12839,7 +12839,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
         <v>828</v>
       </c>
@@ -12874,7 +12874,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
         <v>832</v>
       </c>
@@ -12909,7 +12909,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
         <v>836</v>
       </c>
@@ -12944,7 +12944,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
         <v>840</v>
       </c>
@@ -12979,7 +12979,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
         <v>844</v>
       </c>
@@ -13014,7 +13014,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
         <v>848</v>
       </c>
@@ -13049,7 +13049,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
         <v>852</v>
       </c>
@@ -13084,7 +13084,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
         <v>856</v>
       </c>
@@ -13119,7 +13119,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
         <v>860</v>
       </c>
@@ -13154,7 +13154,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
         <v>864</v>
       </c>
@@ -13189,7 +13189,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
         <v>868</v>
       </c>
@@ -13224,7 +13224,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
         <v>872</v>
       </c>
@@ -13259,7 +13259,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
         <v>876</v>
       </c>
@@ -13294,7 +13294,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
         <v>880</v>
       </c>
@@ -13329,7 +13329,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
         <v>884</v>
       </c>
@@ -13364,7 +13364,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
         <v>888</v>
       </c>
@@ -13399,7 +13399,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
         <v>892</v>
       </c>
@@ -13434,7 +13434,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
         <v>896</v>
       </c>
@@ -13469,7 +13469,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
         <v>900</v>
       </c>
@@ -13504,7 +13504,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
         <v>904</v>
       </c>
@@ -13539,7 +13539,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
         <v>350</v>
       </c>
@@ -13574,7 +13574,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
         <v>911</v>
       </c>
@@ -13609,7 +13609,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
         <v>915</v>
       </c>
@@ -13644,7 +13644,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
         <v>919</v>
       </c>
@@ -13679,7 +13679,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
         <v>923</v>
       </c>
@@ -13714,7 +13714,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
         <v>927</v>
       </c>
@@ -13749,7 +13749,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
         <v>931</v>
       </c>
@@ -13784,7 +13784,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
         <v>935</v>
       </c>
@@ -13819,7 +13819,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
         <v>939</v>
       </c>
@@ -13854,7 +13854,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
         <v>943</v>
       </c>
@@ -13889,7 +13889,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
         <v>947</v>
       </c>
@@ -13924,7 +13924,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
         <v>951</v>
       </c>
@@ -13959,7 +13959,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
         <v>955</v>
       </c>
@@ -13994,7 +13994,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
         <v>959</v>
       </c>
@@ -14029,7 +14029,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
         <v>963</v>
       </c>
@@ -14064,7 +14064,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="236" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
         <v>967</v>
       </c>
@@ -14099,7 +14099,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
         <v>971</v>
       </c>
@@ -14134,7 +14134,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="238" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
         <v>975</v>
       </c>
@@ -14169,7 +14169,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
         <v>979</v>
       </c>
@@ -14204,7 +14204,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
         <v>983</v>
       </c>
@@ -14239,7 +14239,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
         <v>987</v>
       </c>
@@ -14274,7 +14274,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
         <v>991</v>
       </c>
@@ -14309,7 +14309,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
         <v>749</v>
       </c>
@@ -14344,7 +14344,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="244" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
         <v>998</v>
       </c>
@@ -14379,7 +14379,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="245" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
         <v>1002</v>
       </c>
@@ -14414,7 +14414,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
         <v>1006</v>
       </c>
@@ -14449,7 +14449,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="247" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
         <v>1010</v>
       </c>
@@ -14484,7 +14484,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
         <v>1014</v>
       </c>
@@ -14519,7 +14519,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="249" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A249" s="1" t="s">
         <v>362</v>
       </c>
@@ -14554,7 +14554,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A250" s="1" t="s">
         <v>1021</v>
       </c>
@@ -14589,7 +14589,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A251" s="1" t="s">
         <v>1025</v>
       </c>
@@ -14624,7 +14624,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="252" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A252" s="1" t="s">
         <v>1029</v>
       </c>
@@ -14659,7 +14659,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="253" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A253" s="1" t="s">
         <v>1033</v>
       </c>
@@ -14694,7 +14694,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="254" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A254" s="1" t="s">
         <v>1037</v>
       </c>
@@ -14729,7 +14729,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="255" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A255" s="1" t="s">
         <v>1041</v>
       </c>
@@ -14764,7 +14764,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A256" s="1" t="s">
         <v>1045</v>
       </c>
@@ -14799,7 +14799,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="257" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A257" s="1" t="s">
         <v>1049</v>
       </c>
@@ -14834,7 +14834,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="258" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A258" s="1" t="s">
         <v>1053</v>
       </c>
@@ -14869,7 +14869,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="259" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A259" s="1" t="s">
         <v>1057</v>
       </c>
@@ -14904,7 +14904,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="260" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A260" s="1" t="s">
         <v>1061</v>
       </c>
@@ -14939,7 +14939,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="261" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A261" s="1" t="s">
         <v>1065</v>
       </c>
@@ -14974,7 +14974,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="262" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A262" s="1" t="s">
         <v>1069</v>
       </c>
@@ -15009,7 +15009,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="263" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A263" s="1" t="s">
         <v>1073</v>
       </c>
@@ -15044,7 +15044,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="264" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A264" s="1" t="s">
         <v>1077</v>
       </c>
@@ -15079,7 +15079,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="265" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A265" s="1" t="s">
         <v>632</v>
       </c>
@@ -15114,7 +15114,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="266" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A266" s="1" t="s">
         <v>1084</v>
       </c>
@@ -15149,7 +15149,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="267" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A267" s="1" t="s">
         <v>892</v>
       </c>
@@ -15184,7 +15184,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="268" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A268" s="1" t="s">
         <v>1091</v>
       </c>
@@ -15219,7 +15219,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="269" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A269" s="1" t="s">
         <v>1095</v>
       </c>
@@ -15254,7 +15254,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A270" s="1" t="s">
         <v>470</v>
       </c>
@@ -15289,7 +15289,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="271" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A271" s="1" t="s">
         <v>1102</v>
       </c>
@@ -15324,7 +15324,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="272" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A272" s="1" t="s">
         <v>1106</v>
       </c>
@@ -15359,7 +15359,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A273" s="1" t="s">
         <v>1110</v>
       </c>
@@ -15394,7 +15394,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A274" s="1" t="s">
         <v>1114</v>
       </c>
@@ -15429,7 +15429,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A275" s="1" t="s">
         <v>1118</v>
       </c>
@@ -15464,7 +15464,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A276" s="1" t="s">
         <v>433</v>
       </c>
@@ -15499,7 +15499,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A277" s="1" t="s">
         <v>1125</v>
       </c>
@@ -15534,7 +15534,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A278" s="1" t="s">
         <v>1129</v>
       </c>
@@ -15569,7 +15569,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A279" s="1" t="s">
         <v>1133</v>
       </c>
@@ -15604,7 +15604,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A280" s="1" t="s">
         <v>1137</v>
       </c>
@@ -15639,7 +15639,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A281" s="1" t="s">
         <v>1141</v>
       </c>
@@ -15674,7 +15674,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A282" s="1" t="s">
         <v>1145</v>
       </c>
@@ -15709,7 +15709,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="283" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A283" s="1" t="s">
         <v>1149</v>
       </c>
@@ -15744,7 +15744,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A284" s="1" t="s">
         <v>1153</v>
       </c>
@@ -15779,7 +15779,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="285" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A285" s="1" t="s">
         <v>1157</v>
       </c>
@@ -15814,7 +15814,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="286" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A286" s="1" t="s">
         <v>1161</v>
       </c>
@@ -15849,7 +15849,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="287" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A287" s="1" t="s">
         <v>1165</v>
       </c>
@@ -15884,7 +15884,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="288" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A288" s="1" t="s">
         <v>1169</v>
       </c>
@@ -15919,7 +15919,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="289" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A289" s="1" t="s">
         <v>998</v>
       </c>
@@ -15954,7 +15954,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="290" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A290" s="1" t="s">
         <v>1176</v>
       </c>
@@ -15989,7 +15989,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="291" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A291" s="1" t="s">
         <v>1180</v>
       </c>
@@ -16024,7 +16024,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="292" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A292" s="1" t="s">
         <v>1184</v>
       </c>
@@ -16059,7 +16059,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="293" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A293" s="1" t="s">
         <v>1188</v>
       </c>
@@ -16094,7 +16094,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="294" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A294" s="1" t="s">
         <v>1192</v>
       </c>
@@ -16129,7 +16129,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="295" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A295" s="1" t="s">
         <v>1091</v>
       </c>
@@ -16164,7 +16164,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="296" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A296" s="1" t="s">
         <v>1199</v>
       </c>
@@ -16199,7 +16199,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="297" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A297" s="1" t="s">
         <v>1203</v>
       </c>
@@ -16234,7 +16234,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="298" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A298" s="1" t="s">
         <v>1207</v>
       </c>
@@ -16269,7 +16269,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="299" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A299" s="1" t="s">
         <v>1211</v>
       </c>
@@ -16304,7 +16304,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="300" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A300" s="1" t="s">
         <v>1215</v>
       </c>
@@ -16339,7 +16339,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="301" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A301" s="1" t="s">
         <v>659</v>
       </c>
@@ -16374,7 +16374,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="302" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A302" s="1" t="s">
         <v>1222</v>
       </c>
@@ -16409,7 +16409,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="303" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A303" s="1" t="s">
         <v>1226</v>
       </c>
@@ -16444,7 +16444,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="304" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A304" s="1" t="s">
         <v>1230</v>
       </c>
@@ -16479,7 +16479,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="305" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A305" s="1" t="s">
         <v>1234</v>
       </c>
@@ -16514,7 +16514,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="306" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A306" s="1" t="s">
         <v>1238</v>
       </c>
@@ -16549,7 +16549,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="307" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A307" s="1" t="s">
         <v>1242</v>
       </c>
@@ -16584,7 +16584,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="308" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A308" s="1" t="s">
         <v>753</v>
       </c>
@@ -16619,7 +16619,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="309" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A309" s="1" t="s">
         <v>1249</v>
       </c>
@@ -16654,7 +16654,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="310" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A310" s="1" t="s">
         <v>1253</v>
       </c>
@@ -16689,7 +16689,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="311" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A311" s="1" t="s">
         <v>1258</v>
       </c>
@@ -16724,7 +16724,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="312" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A312" s="1" t="s">
         <v>1261</v>
       </c>
@@ -16759,7 +16759,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="313" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A313" s="1" t="s">
         <v>1264</v>
       </c>
@@ -16794,7 +16794,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="314" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A314" s="1" t="s">
         <v>1267</v>
       </c>
@@ -16829,7 +16829,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="315" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A315" s="1" t="s">
         <v>1270</v>
       </c>
@@ -16864,7 +16864,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="316" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A316" s="1" t="s">
         <v>1273</v>
       </c>
@@ -16899,7 +16899,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="317" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A317" s="1" t="s">
         <v>1276</v>
       </c>
@@ -16934,7 +16934,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="318" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A318" s="1" t="s">
         <v>1279</v>
       </c>
@@ -16969,7 +16969,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="319" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A319" s="1" t="s">
         <v>1282</v>
       </c>
@@ -17004,7 +17004,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="320" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A320" s="1" t="s">
         <v>1285</v>
       </c>
@@ -17039,7 +17039,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="321" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A321" s="1" t="s">
         <v>550</v>
       </c>
@@ -17074,7 +17074,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="322" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A322" s="1" t="s">
         <v>1290</v>
       </c>
@@ -17109,7 +17109,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="323" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A323" s="1" t="s">
         <v>1293</v>
       </c>
@@ -17144,7 +17144,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="324" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A324" s="1" t="s">
         <v>1296</v>
       </c>
@@ -17179,7 +17179,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="325" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A325" s="1" t="s">
         <v>1299</v>
       </c>
@@ -17214,7 +17214,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="326" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A326" s="1" t="s">
         <v>1302</v>
       </c>
@@ -17249,7 +17249,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="327" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A327" s="1" t="s">
         <v>1305</v>
       </c>
@@ -17284,7 +17284,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="328" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A328" s="1" t="s">
         <v>1308</v>
       </c>
@@ -17319,7 +17319,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="329" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A329" s="1" t="s">
         <v>1311</v>
       </c>
@@ -17354,7 +17354,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="330" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A330" s="1" t="s">
         <v>1314</v>
       </c>
@@ -17389,7 +17389,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="331" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A331" s="1" t="s">
         <v>1317</v>
       </c>
@@ -17424,7 +17424,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="332" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A332" s="1" t="s">
         <v>1320</v>
       </c>
@@ -17459,7 +17459,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="333" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A333" s="1" t="s">
         <v>1323</v>
       </c>
@@ -17494,7 +17494,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="334" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A334" s="1" t="s">
         <v>1326</v>
       </c>
@@ -17529,7 +17529,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="335" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A335" s="1" t="s">
         <v>1329</v>
       </c>
@@ -17564,7 +17564,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="336" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A336" s="1" t="s">
         <v>1332</v>
       </c>
@@ -17599,7 +17599,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="337" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A337" s="1" t="s">
         <v>1335</v>
       </c>
@@ -17634,7 +17634,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="338" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A338" s="1" t="s">
         <v>852</v>
       </c>
@@ -17669,7 +17669,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="339" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A339" s="1" t="s">
         <v>1340</v>
       </c>
@@ -17704,7 +17704,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="340" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A340" s="1" t="s">
         <v>1343</v>
       </c>
@@ -17739,7 +17739,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="341" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A341" s="1" t="s">
         <v>1199</v>
       </c>
@@ -17774,7 +17774,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="342" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A342" s="1" t="s">
         <v>1348</v>
       </c>
@@ -17809,7 +17809,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="343" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A343" s="1" t="s">
         <v>482</v>
       </c>
@@ -17844,7 +17844,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="344" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A344" s="1" t="s">
         <v>1353</v>
       </c>
@@ -17879,7 +17879,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="345" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A345" s="1" t="s">
         <v>1356</v>
       </c>
@@ -17914,7 +17914,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="346" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A346" s="1" t="s">
         <v>1359</v>
       </c>
@@ -17949,7 +17949,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="347" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A347" s="1" t="s">
         <v>108</v>
       </c>
@@ -17984,7 +17984,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="348" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A348" s="1" t="s">
         <v>1364</v>
       </c>
@@ -18019,7 +18019,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="349" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A349" s="1" t="s">
         <v>1367</v>
       </c>
@@ -18054,7 +18054,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="350" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A350" s="1" t="s">
         <v>1370</v>
       </c>
@@ -18089,7 +18089,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="351" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A351" s="1" t="s">
         <v>1373</v>
       </c>
@@ -18124,7 +18124,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="352" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A352" s="1" t="s">
         <v>741</v>
       </c>
@@ -18159,7 +18159,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="353" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A353" s="1" t="s">
         <v>1378</v>
       </c>
@@ -18194,7 +18194,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="354" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A354" s="1" t="s">
         <v>506</v>
       </c>
@@ -18229,7 +18229,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="355" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A355" s="1" t="s">
         <v>1383</v>
       </c>
@@ -18264,7 +18264,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="356" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A356" s="1" t="s">
         <v>1386</v>
       </c>
@@ -18299,7 +18299,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="357" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A357" s="1" t="s">
         <v>1389</v>
       </c>
@@ -18334,7 +18334,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="358" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A358" s="1" t="s">
         <v>1392</v>
       </c>
@@ -18369,7 +18369,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="359" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A359" s="1" t="s">
         <v>252</v>
       </c>
@@ -18404,7 +18404,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="360" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A360" s="1" t="s">
         <v>1397</v>
       </c>
@@ -18439,7 +18439,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="361" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A361" s="1" t="s">
         <v>1400</v>
       </c>
@@ -18474,7 +18474,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="362" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A362" s="1" t="s">
         <v>1403</v>
       </c>
@@ -18509,7 +18509,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="363" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A363" s="1" t="s">
         <v>269</v>
       </c>
@@ -18544,7 +18544,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="364" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A364" s="1" t="s">
         <v>1408</v>
       </c>
@@ -18579,7 +18579,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="365" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A365" s="1" t="s">
         <v>1411</v>
       </c>
@@ -18614,7 +18614,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="366" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A366" s="1" t="s">
         <v>1414</v>
       </c>
@@ -18649,7 +18649,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="367" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A367" s="1" t="s">
         <v>298</v>
       </c>
@@ -18684,7 +18684,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="368" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A368" s="1" t="s">
         <v>1419</v>
       </c>
@@ -18719,7 +18719,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="369" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A369" s="1" t="s">
         <v>1422</v>
       </c>
@@ -18754,7 +18754,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="370" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A370" s="1" t="s">
         <v>1425</v>
       </c>
@@ -18789,7 +18789,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="371" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A371" s="1" t="s">
         <v>1428</v>
       </c>
@@ -18824,7 +18824,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="372" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A372" s="1" t="s">
         <v>1431</v>
       </c>
@@ -18859,7 +18859,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="373" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A373" s="1" t="s">
         <v>1434</v>
       </c>
@@ -18894,7 +18894,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="374" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A374" s="1" t="s">
         <v>186</v>
       </c>
@@ -18929,7 +18929,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="375" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A375" s="1" t="s">
         <v>693</v>
       </c>
@@ -18964,7 +18964,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="376" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A376" s="1" t="s">
         <v>318</v>
       </c>
@@ -18999,7 +18999,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="377" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A377" s="1" t="s">
         <v>1443</v>
       </c>
@@ -19034,7 +19034,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="378" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A378" s="1" t="s">
         <v>1446</v>
       </c>
@@ -19069,7 +19069,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="379" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A379" s="1" t="s">
         <v>1449</v>
       </c>
@@ -19104,7 +19104,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="380" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A380" s="1" t="s">
         <v>1452</v>
       </c>
@@ -19139,7 +19139,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="381" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A381" s="1" t="s">
         <v>1455</v>
       </c>
@@ -19174,7 +19174,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="382" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A382" s="1" t="s">
         <v>1458</v>
       </c>
@@ -19209,7 +19209,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="383" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A383" s="1" t="s">
         <v>1461</v>
       </c>
@@ -19244,7 +19244,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="384" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A384" s="1" t="s">
         <v>1464</v>
       </c>
@@ -19279,7 +19279,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="385" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A385" s="1" t="s">
         <v>1467</v>
       </c>
@@ -19314,7 +19314,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="386" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A386" s="1" t="s">
         <v>1470</v>
       </c>
@@ -19349,7 +19349,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="387" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A387" s="1" t="s">
         <v>1473</v>
       </c>
@@ -19384,7 +19384,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="388" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A388" s="1" t="s">
         <v>1476</v>
       </c>
@@ -19419,7 +19419,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="389" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A389" s="1" t="s">
         <v>1479</v>
       </c>
@@ -19454,7 +19454,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="390" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A390" s="1" t="s">
         <v>1482</v>
       </c>
@@ -19489,7 +19489,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="391" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A391" s="1" t="s">
         <v>1485</v>
       </c>
@@ -19524,7 +19524,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="392" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A392" s="1" t="s">
         <v>1488</v>
       </c>
@@ -19559,7 +19559,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="393" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A393" s="1" t="s">
         <v>1491</v>
       </c>
@@ -19594,7 +19594,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="394" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A394" s="1" t="s">
         <v>1494</v>
       </c>
@@ -19629,7 +19629,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="395" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A395" s="1" t="s">
         <v>1497</v>
       </c>
@@ -19664,7 +19664,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="396" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A396" s="1" t="s">
         <v>1500</v>
       </c>
@@ -19699,7 +19699,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="397" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A397" s="1" t="s">
         <v>1503</v>
       </c>
@@ -19734,7 +19734,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="398" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A398" s="1" t="s">
         <v>1506</v>
       </c>
@@ -19769,7 +19769,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="399" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A399" s="1" t="s">
         <v>1509</v>
       </c>
@@ -19804,7 +19804,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="400" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A400" s="1" t="s">
         <v>1512</v>
       </c>
@@ -19839,7 +19839,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="401" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A401" s="1" t="s">
         <v>1515</v>
       </c>
@@ -19874,7 +19874,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="402" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A402" s="1" t="s">
         <v>1518</v>
       </c>
@@ -19909,7 +19909,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="403" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A403" s="1" t="s">
         <v>1521</v>
       </c>
@@ -19944,7 +19944,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="404" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A404" s="1" t="s">
         <v>1524</v>
       </c>
@@ -19979,7 +19979,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="405" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A405" s="1" t="s">
         <v>1527</v>
       </c>
@@ -20014,7 +20014,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="406" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A406" s="1" t="s">
         <v>1530</v>
       </c>
@@ -20049,7 +20049,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="407" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A407" s="1" t="s">
         <v>1533</v>
       </c>
@@ -20084,7 +20084,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="408" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A408" s="1" t="s">
         <v>1536</v>
       </c>
@@ -20119,7 +20119,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="409" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A409" s="1" t="s">
         <v>1539</v>
       </c>
@@ -20154,7 +20154,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="410" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A410" s="1" t="s">
         <v>1542</v>
       </c>
@@ -20189,7 +20189,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="411" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A411" s="1" t="s">
         <v>1545</v>
       </c>
@@ -20224,7 +20224,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="412" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A412" s="1" t="s">
         <v>1548</v>
       </c>
@@ -20259,7 +20259,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="413" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A413" s="1" t="s">
         <v>1551</v>
       </c>
@@ -20294,7 +20294,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="414" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A414" s="1" t="s">
         <v>1554</v>
       </c>
@@ -20329,7 +20329,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="415" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A415" s="1" t="s">
         <v>1557</v>
       </c>
@@ -20364,7 +20364,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="416" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A416" s="1" t="s">
         <v>1560</v>
       </c>
@@ -20399,7 +20399,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="417" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A417" s="1" t="s">
         <v>1563</v>
       </c>
@@ -20434,7 +20434,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="418" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A418" s="1" t="s">
         <v>178</v>
       </c>
@@ -20469,7 +20469,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="419" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A419" s="1" t="s">
         <v>1568</v>
       </c>
@@ -20504,7 +20504,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="420" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A420" s="1" t="s">
         <v>1571</v>
       </c>
@@ -20539,7 +20539,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="421" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A421" s="1" t="s">
         <v>1574</v>
       </c>
@@ -20574,7 +20574,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="422" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A422" s="1" t="s">
         <v>1577</v>
       </c>
@@ -20609,7 +20609,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="423" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A423" s="1" t="s">
         <v>1580</v>
       </c>
@@ -20644,7 +20644,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="424" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A424" s="1" t="s">
         <v>1583</v>
       </c>
@@ -20679,7 +20679,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="425" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A425" s="1" t="s">
         <v>1586</v>
       </c>
@@ -20714,7 +20714,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="426" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A426" s="1" t="s">
         <v>1589</v>
       </c>
@@ -20749,7 +20749,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="427" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A427" s="1" t="s">
         <v>1592</v>
       </c>
@@ -20784,7 +20784,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="428" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A428" s="1" t="s">
         <v>1595</v>
       </c>
@@ -20819,7 +20819,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="429" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A429" s="1" t="s">
         <v>1598</v>
       </c>
@@ -20854,7 +20854,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="430" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A430" s="1" t="s">
         <v>1601</v>
       </c>
@@ -20889,7 +20889,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="431" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A431" s="1" t="s">
         <v>1604</v>
       </c>
@@ -20924,7 +20924,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="432" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A432" s="1" t="s">
         <v>1607</v>
       </c>
@@ -20959,7 +20959,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="433" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A433" s="1" t="s">
         <v>366</v>
       </c>
@@ -20994,7 +20994,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="434" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A434" s="1" t="s">
         <v>1612</v>
       </c>
@@ -21029,7 +21029,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="435" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A435" s="1" t="s">
         <v>1615</v>
       </c>
@@ -21064,7 +21064,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="436" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A436" s="1" t="s">
         <v>1618</v>
       </c>
@@ -21099,7 +21099,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="437" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A437" s="1" t="s">
         <v>1621</v>
       </c>
@@ -21134,7 +21134,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="438" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A438" s="1" t="s">
         <v>1624</v>
       </c>
@@ -21169,7 +21169,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="439" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A439" s="1" t="s">
         <v>334</v>
       </c>
@@ -21204,7 +21204,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="440" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A440" s="1" t="s">
         <v>1629</v>
       </c>
@@ -21239,7 +21239,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="441" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A441" s="1" t="s">
         <v>1378</v>
       </c>
@@ -21274,7 +21274,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="442" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A442" s="1" t="s">
         <v>904</v>
       </c>
@@ -21309,7 +21309,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="443" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A443" s="1" t="s">
         <v>1636</v>
       </c>
@@ -21344,7 +21344,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="444" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A444" s="1" t="s">
         <v>1639</v>
       </c>
@@ -21379,7 +21379,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="445" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A445" s="1" t="s">
         <v>1642</v>
       </c>
@@ -21414,7 +21414,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="446" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A446" s="1" t="s">
         <v>852</v>
       </c>
@@ -21449,7 +21449,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="447" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="447" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A447" s="1" t="s">
         <v>1647</v>
       </c>
@@ -21484,7 +21484,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="448" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="448" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A448" s="1" t="s">
         <v>502</v>
       </c>
@@ -21519,7 +21519,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="449" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="449" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A449" s="1" t="s">
         <v>1652</v>
       </c>
@@ -21554,7 +21554,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="450" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="450" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A450" s="1" t="s">
         <v>1655</v>
       </c>
@@ -21589,7 +21589,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="451" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="451" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A451" s="1" t="s">
         <v>1658</v>
       </c>
@@ -21624,7 +21624,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="452" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="452" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A452" s="1" t="s">
         <v>1661</v>
       </c>
@@ -21659,7 +21659,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="453" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="453" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A453" s="1" t="s">
         <v>244</v>
       </c>
@@ -21694,7 +21694,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="454" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="454" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A454" s="1" t="s">
         <v>1666</v>
       </c>
@@ -21729,7 +21729,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="455" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="455" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A455" s="1" t="s">
         <v>1669</v>
       </c>
@@ -21764,7 +21764,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="456" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="456" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A456" s="1" t="s">
         <v>1672</v>
       </c>
@@ -21799,7 +21799,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="457" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="457" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A457" s="1" t="s">
         <v>1675</v>
       </c>
@@ -21834,7 +21834,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="458" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="458" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A458" s="1" t="s">
         <v>1021</v>
       </c>
@@ -21869,7 +21869,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="459" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="459" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A459" s="1" t="s">
         <v>1680</v>
       </c>
@@ -21904,7 +21904,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="460" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="460" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A460" s="1" t="s">
         <v>1683</v>
       </c>
@@ -21939,7 +21939,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="461" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="461" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A461" s="1" t="s">
         <v>1686</v>
       </c>
@@ -21974,7 +21974,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="462" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="462" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A462" s="1" t="s">
         <v>1689</v>
       </c>
@@ -22009,7 +22009,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="463" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="463" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A463" s="1" t="s">
         <v>1692</v>
       </c>
@@ -22044,7 +22044,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="464" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="464" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A464" s="1" t="s">
         <v>1695</v>
       </c>
@@ -22079,7 +22079,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="465" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="465" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A465" s="1" t="s">
         <v>1698</v>
       </c>
@@ -22114,7 +22114,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="466" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="466" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A466" s="1" t="s">
         <v>1701</v>
       </c>
@@ -22149,7 +22149,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="467" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="467" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A467" s="1" t="s">
         <v>1704</v>
       </c>
@@ -22184,7 +22184,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="468" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="468" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A468" s="1" t="s">
         <v>991</v>
       </c>
@@ -22219,7 +22219,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="469" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="469" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A469" s="1" t="s">
         <v>1709</v>
       </c>
@@ -22254,7 +22254,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="470" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="470" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A470" s="1" t="s">
         <v>1712</v>
       </c>
@@ -22289,7 +22289,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="471" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="471" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A471" s="1" t="s">
         <v>1715</v>
       </c>
@@ -22324,7 +22324,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="472" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="472" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A472" s="1" t="s">
         <v>1718</v>
       </c>
@@ -22359,7 +22359,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="473" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="473" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A473" s="1" t="s">
         <v>1721</v>
       </c>
@@ -22394,7 +22394,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="474" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="474" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A474" s="1" t="s">
         <v>1724</v>
       </c>
@@ -22429,7 +22429,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="475" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="475" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A475" s="1" t="s">
         <v>1727</v>
       </c>
@@ -22464,7 +22464,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="476" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="476" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A476" s="1" t="s">
         <v>1730</v>
       </c>
@@ -22499,7 +22499,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="477" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="477" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A477" s="1" t="s">
         <v>1733</v>
       </c>
@@ -22534,7 +22534,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="478" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="478" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A478" s="1" t="s">
         <v>1736</v>
       </c>
@@ -22569,7 +22569,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="479" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="479" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A479" s="1" t="s">
         <v>1739</v>
       </c>
@@ -22604,7 +22604,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="480" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="480" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A480" s="1" t="s">
         <v>643</v>
       </c>
@@ -22639,7 +22639,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="481" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="481" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A481" s="1" t="s">
         <v>1744</v>
       </c>
@@ -22674,7 +22674,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="482" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="482" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A482" s="1" t="s">
         <v>1747</v>
       </c>
@@ -22709,7 +22709,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="483" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="483" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A483" s="1" t="s">
         <v>1750</v>
       </c>
@@ -22744,7 +22744,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="484" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="484" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A484" s="1" t="s">
         <v>1666</v>
       </c>
@@ -22779,7 +22779,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="485" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="485" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A485" s="1" t="s">
         <v>1755</v>
       </c>
@@ -22814,7 +22814,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="486" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="486" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A486" s="1" t="s">
         <v>1758</v>
       </c>
@@ -22849,7 +22849,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="487" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="487" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A487" s="1" t="s">
         <v>1761</v>
       </c>
@@ -22884,7 +22884,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="488" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="488" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A488" s="1" t="s">
         <v>1764</v>
       </c>
@@ -22919,7 +22919,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="489" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="489" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A489" s="1" t="s">
         <v>1767</v>
       </c>
@@ -22954,7 +22954,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="490" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="490" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A490" s="1" t="s">
         <v>1770</v>
       </c>
@@ -22989,7 +22989,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="491" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="491" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A491" s="1" t="s">
         <v>1773</v>
       </c>
@@ -23024,7 +23024,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="492" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="492" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A492" s="1" t="s">
         <v>836</v>
       </c>
@@ -23059,7 +23059,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="493" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="493" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A493" s="1" t="s">
         <v>1411</v>
       </c>
@@ -23094,7 +23094,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="494" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="494" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A494" s="1" t="s">
         <v>1780</v>
       </c>
@@ -23129,7 +23129,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="495" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="495" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A495" s="1" t="s">
         <v>1783</v>
       </c>
@@ -23164,7 +23164,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="496" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="496" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A496" s="1" t="s">
         <v>1786</v>
       </c>
@@ -23199,7 +23199,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="497" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="497" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A497" s="1" t="s">
         <v>1789</v>
       </c>
@@ -23234,7 +23234,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="498" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="498" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A498" s="1" t="s">
         <v>1792</v>
       </c>
@@ -23269,7 +23269,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="499" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="499" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A499" s="1" t="s">
         <v>1795</v>
       </c>
@@ -23304,7 +23304,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="500" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="500" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A500" s="1" t="s">
         <v>1798</v>
       </c>
@@ -23339,7 +23339,7 @@
         <v>1257</v>
       </c>
     </row>
-    <row r="501" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="501" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A501" s="1" t="s">
         <v>1801</v>
       </c>

</xml_diff>